<commit_message>
Monte Carlo finished! :)
</commit_message>
<xml_diff>
--- a/Risk Driver Simulation/Input/Correlation/correlationmatrix.xlsx
+++ b/Risk Driver Simulation/Input/Correlation/correlationmatrix.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Risk Driver Simulation\Input\Correlation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F2A6DE-5833-4B1A-88BA-06336381F63A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
+    <workbookView xWindow="-28920" yWindow="-6465" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,33 +22,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>EUR</t>
-  </si>
-  <si>
-    <t>GBP</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>EURGBP</t>
-  </si>
-  <si>
     <t>EURUSD</t>
-  </si>
-  <si>
-    <t>EURJPY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,6 +78,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -132,7 +129,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -165,9 +162,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,6 +214,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -375,219 +406,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-0.44989699999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3.3731999999999998E-2</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.11050416534731369</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.19007270732067019</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3.4670374212956878E-2</v>
-      </c>
-      <c r="F2" s="1">
-        <v>-6.98607774530971E-2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>-8.5185640792035597E-2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>8.0908258938299019E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="1">
+        <v>-0.44989699999999999</v>
+      </c>
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.11050416534731369</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.99999999999999989</v>
-      </c>
       <c r="D3" s="1">
-        <v>-8.6122247422535922E-2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-4.3300304878417011E-2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.1537703601515292</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.1535004234025511</v>
-      </c>
-      <c r="H3" s="1">
-        <v>6.1425054869273021E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.113924</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>0.19007270732067019</v>
+        <v>3.3731999999999998E-2</v>
       </c>
       <c r="C4" s="1">
-        <v>-8.6122247422535866E-2</v>
+        <v>0.113924</v>
       </c>
       <c r="D4" s="1">
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="E4" s="1">
-        <v>-0.1125279935347195</v>
-      </c>
-      <c r="F4" s="1">
-        <v>-7.7030743627001762E-3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>-2.4097922284645489E-2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>-0.21897359255415949</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3.467037421295692E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-4.3300304878416983E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-0.1125279935347195</v>
-      </c>
-      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
-        <v>3.9193678808130412E-2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>-0.10523140061857671</v>
-      </c>
-      <c r="H5" s="1">
-        <v>-7.3170958566663056E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>-6.9860777453097087E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.15377036015152909</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-7.703074362700079E-3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3.9193678808130412E-2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>4.9410933775471219E-2</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.1437585006432687</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>-8.5185640792035541E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.15350042340255099</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-2.4097922284645489E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-0.10523140061857671</v>
-      </c>
-      <c r="F7" s="1">
-        <v>4.941093377547124E-2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.27291002900796651</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>8.0908258938299032E-2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>6.1425054869272938E-2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>-0.21897359255415949</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-7.3170958566662909E-3</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.1437585006432687</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.27291002900796663</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.99999999999999956</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -595,24 +522,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>